<commit_message>
Date and Time added to Share Skill
</commit_message>
<xml_diff>
--- a/Mars_Competition_Task/Spreadsheets/Share Skill Test Data.xlsx
+++ b/Mars_Competition_Task/Spreadsheets/Share Skill Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankur\Desktop\Mars_Competition_Task\Mars_Competition_Task\Mars_Competition_Task\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34E7F0F-1326-4735-B60B-9BA0241C9C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F8127E-3610-41C2-B2FB-4720E95E5E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8FC286E2-47C3-4669-B831-8C688DB29DD5}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="105">
   <si>
     <t>Title</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>Hourly</t>
+  </si>
+  <si>
+    <t>credit</t>
   </si>
 </sst>
 </file>
@@ -748,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9D9EBF2-48A5-480E-A780-DF45727B18CC}">
   <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -760,8 +763,7 @@
     <col min="4" max="4" width="20.1796875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1796875" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.36328125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="10.08984375" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.6328125" style="4" bestFit="1" customWidth="1"/>
@@ -914,18 +916,18 @@
         <v>48</v>
       </c>
       <c r="C2" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="4" t="str">
         <f>VLOOKUP(C2,Sheet1!$A$9:$B$16,2,0)</f>
-        <v>Programming &amp; Tech</v>
+        <v>Music &amp; Audio</v>
       </c>
       <c r="E2" s="4">
         <v>1</v>
       </c>
       <c r="F2" s="4" t="str">
         <f>VLOOKUP(CONCATENATE(C2,".",E2),Sheet2!$A:$C,3,0)</f>
-        <v>WordPress</v>
+        <v>Mixing &amp; Mastering</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>5</v>
@@ -961,7 +963,7 @@
         <v>102</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>101</v>
@@ -970,7 +972,7 @@
         <v>102</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>101</v>
@@ -1012,7 +1014,7 @@
         <v>61</v>
       </c>
       <c r="AI2" s="8">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="AJ2" s="4" t="s">
         <v>6</v>
@@ -1127,7 +1129,7 @@
         <v>64</v>
       </c>
       <c r="AI3" s="8">
-        <v>124</v>
+        <v>3</v>
       </c>
       <c r="AJ3" s="4" t="s">
         <v>6</v>
@@ -1242,7 +1244,7 @@
         <v>62</v>
       </c>
       <c r="AI4" s="8">
-        <v>125</v>
+        <v>3</v>
       </c>
       <c r="AJ4" s="4" t="s">
         <v>6</v>
@@ -1357,7 +1359,7 @@
         <v>65</v>
       </c>
       <c r="AI5" s="8">
-        <v>126</v>
+        <v>3</v>
       </c>
       <c r="AJ5" s="4" t="s">
         <v>6</v>
@@ -1472,7 +1474,7 @@
         <v>63</v>
       </c>
       <c r="AI6" s="8">
-        <v>127</v>
+        <v>3</v>
       </c>
       <c r="AJ6" s="4" t="s">
         <v>6</v>
@@ -1587,7 +1589,7 @@
         <v>66</v>
       </c>
       <c r="AI7" s="8">
-        <v>128</v>
+        <v>3</v>
       </c>
       <c r="AJ7" s="4" t="s">
         <v>6</v>
@@ -1606,7 +1608,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{09980DCA-9550-4D77-87D6-DF251E2AFFF8}">
           <x14:formula1>
             <xm:f>Sheet1!$A$4:$A$5</xm:f>
@@ -1649,6 +1651,12 @@
           </x14:formula1>
           <xm:sqref>E2:E7</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DBE0D7A-BE48-4437-B0FB-FDBB75E228B3}">
+          <x14:formula1>
+            <xm:f>Sheet1!$F$10:$F$19</xm:f>
+          </x14:formula1>
+          <xm:sqref>AI2:AI7</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1660,7 +1668,7 @@
   <dimension ref="A1:L1444"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F10" sqref="F10:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1818,6 +1826,9 @@
       <c r="D9" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="F9" t="s">
+        <v>104</v>
+      </c>
       <c r="I9">
         <v>0</v>
       </c>
@@ -1845,6 +1856,9 @@
       <c r="D10" s="3" t="s">
         <v>76</v>
       </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
       <c r="I10">
         <v>0</v>
       </c>
@@ -1872,6 +1886,9 @@
       <c r="D11" s="3" t="s">
         <v>77</v>
       </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
       <c r="I11">
         <v>0</v>
       </c>
@@ -1899,6 +1916,9 @@
       <c r="D12" s="3" t="s">
         <v>78</v>
       </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
       <c r="I12">
         <v>0</v>
       </c>
@@ -1926,6 +1946,9 @@
       <c r="D13" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
       <c r="I13">
         <v>0</v>
       </c>
@@ -1947,6 +1970,9 @@
       <c r="B14" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
       <c r="I14">
         <v>0</v>
       </c>
@@ -1968,6 +1994,9 @@
       <c r="B15" s="3" t="s">
         <v>73</v>
       </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
       <c r="I15">
         <v>0</v>
       </c>
@@ -1989,6 +2018,9 @@
       <c r="B16" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
       <c r="I16">
         <v>0</v>
       </c>
@@ -2003,7 +2035,10 @@
         <v>0:12 AM</v>
       </c>
     </row>
-    <row r="17" spans="9:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F17">
+        <v>7</v>
+      </c>
       <c r="I17">
         <v>0</v>
       </c>
@@ -2018,7 +2053,10 @@
         <v>0:13 AM</v>
       </c>
     </row>
-    <row r="18" spans="9:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F18">
+        <v>8</v>
+      </c>
       <c r="I18">
         <v>0</v>
       </c>
@@ -2033,7 +2071,10 @@
         <v>0:14 AM</v>
       </c>
     </row>
-    <row r="19" spans="9:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F19">
+        <v>9</v>
+      </c>
       <c r="I19">
         <v>0</v>
       </c>
@@ -2048,7 +2089,7 @@
         <v>0:15 AM</v>
       </c>
     </row>
-    <row r="20" spans="9:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="6:12" x14ac:dyDescent="0.35">
       <c r="I20">
         <v>0</v>
       </c>
@@ -2063,7 +2104,7 @@
         <v>0:16 AM</v>
       </c>
     </row>
-    <row r="21" spans="9:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="6:12" x14ac:dyDescent="0.35">
       <c r="I21">
         <v>0</v>
       </c>
@@ -2078,7 +2119,7 @@
         <v>0:17 AM</v>
       </c>
     </row>
-    <row r="22" spans="9:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="6:12" x14ac:dyDescent="0.35">
       <c r="I22">
         <v>0</v>
       </c>
@@ -2093,7 +2134,7 @@
         <v>0:18 AM</v>
       </c>
     </row>
-    <row r="23" spans="9:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="6:12" x14ac:dyDescent="0.35">
       <c r="I23">
         <v>0</v>
       </c>
@@ -2108,7 +2149,7 @@
         <v>0:19 AM</v>
       </c>
     </row>
-    <row r="24" spans="9:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="6:12" x14ac:dyDescent="0.35">
       <c r="I24">
         <v>0</v>
       </c>
@@ -2123,7 +2164,7 @@
         <v>0:20 AM</v>
       </c>
     </row>
-    <row r="25" spans="9:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="6:12" x14ac:dyDescent="0.35">
       <c r="I25">
         <v>0</v>
       </c>
@@ -2138,7 +2179,7 @@
         <v>0:21 AM</v>
       </c>
     </row>
-    <row r="26" spans="9:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="6:12" x14ac:dyDescent="0.35">
       <c r="I26">
         <v>0</v>
       </c>
@@ -2153,7 +2194,7 @@
         <v>0:22 AM</v>
       </c>
     </row>
-    <row r="27" spans="9:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="6:12" x14ac:dyDescent="0.35">
       <c r="I27">
         <v>0</v>
       </c>
@@ -2168,7 +2209,7 @@
         <v>0:23 AM</v>
       </c>
     </row>
-    <row r="28" spans="9:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="6:12" x14ac:dyDescent="0.35">
       <c r="I28">
         <v>0</v>
       </c>
@@ -2183,7 +2224,7 @@
         <v>0:24 AM</v>
       </c>
     </row>
-    <row r="29" spans="9:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="6:12" x14ac:dyDescent="0.35">
       <c r="I29">
         <v>0</v>
       </c>
@@ -2198,7 +2239,7 @@
         <v>0:25 AM</v>
       </c>
     </row>
-    <row r="30" spans="9:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="6:12" x14ac:dyDescent="0.35">
       <c r="I30">
         <v>0</v>
       </c>
@@ -2213,7 +2254,7 @@
         <v>0:26 AM</v>
       </c>
     </row>
-    <row r="31" spans="9:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="6:12" x14ac:dyDescent="0.35">
       <c r="I31">
         <v>0</v>
       </c>
@@ -2228,7 +2269,7 @@
         <v>0:27 AM</v>
       </c>
     </row>
-    <row r="32" spans="9:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="6:12" x14ac:dyDescent="0.35">
       <c r="I32">
         <v>0</v>
       </c>
@@ -26083,7 +26124,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:A31"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>